<commit_message>
add links to notes and notebooks
</commit_message>
<xml_diff>
--- a/content/writing/data-raw/writings.xlsx
+++ b/content/writing/data-raw/writings.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>title</t>
   </si>
@@ -32,22 +32,55 @@
     <t>finished</t>
   </si>
   <si>
+    <t>Completing KF-SPLS with Ryser</t>
+  </si>
+  <si>
+    <t>An [IPython][ipython] notebook demonstrating some ideas about completing KF-SPLS using the [Ryser][ryserhome] package for partial latin square completion.</t>
+  </si>
+  <si>
+    <t>An Introduction to NetworkX</t>
+  </si>
+  <si>
+    <t>An IPython notebook demonstrating the use of the NetworkX package for graph and network analysis in Python</t>
+  </si>
+  <si>
+    <t>Computational and Numerical Methods</t>
+  </si>
+  <si>
+    <t>An IPython notebook demonstrating the use of Octave for numerical methods.</t>
+  </si>
+  <si>
+    <t>Processing GPS Data in Python</t>
+  </si>
+  <si>
+    <t>An [IPython][ipython] notebook presenting a statistical investigation, based on GPS data, into anomalous driving patterns among a fleet of delivery trucks</t>
+  </si>
+  <si>
+    <t>Modelling Sudoku Puzzles in Python</t>
+  </si>
+  <si>
+    <t>An updated version of {% cite davis7modeling –file mh2 %} as an IPython notebook.</t>
+  </si>
+  <si>
+    <t>Speech Annotation in Python Using Regular Expressions</t>
+  </si>
+  <si>
+    <t>An IPython notebook which illustrates some basic ideas about annotating a corpus of novels using regular expressions.</t>
+  </si>
+  <si>
+    <t>List-colouring in Python with Vizing</t>
+  </si>
+  <si>
+    <t>An IPython notebook introducing list-colouring of graphs using the [Vizing][vizinghome] package.</t>
+  </si>
+  <si>
     <t>On Polytopes and Lattice-Point Enumeration</t>
   </si>
   <si>
-    <t>Completing KF-SPLS with Ryser</t>
-  </si>
-  <si>
     <t>Some notes on Ehrhart Theory, particularly on using Polymake.</t>
   </si>
   <si>
-    <t>An [IPython][ipython] notebook demonstrating some ideas about completing KF-SPLS using the [Ryser][ryserhome] package for partial latin square completion.</t>
-  </si>
-  <si>
-    <t>An Introduction to NetworkX</t>
-  </si>
-  <si>
-    <t>An IPython notebook demonstrating the use of the NetworkX package for graph and network analysis in Python</t>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/14_03_09_ehrhart.pdf</t>
   </si>
   <si>
     <t>On the Completability of Wing-Form Partial Latin Squares</t>
@@ -56,10 +89,7 @@
     <t>An article about completing WF-SPLS in which the completable, bound, untethered KF-SPLS of even order are characterised.</t>
   </si>
   <si>
-    <t>Computational and Numerical Methods</t>
-  </si>
-  <si>
-    <t>An IPython notebook demonstrating the use of Octave for numerical methods.</t>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/13_06_28_wingform.pdf</t>
   </si>
   <si>
     <t>Some Observations on the Intricacy of Partial Latin Square Completion</t>
@@ -68,22 +98,7 @@
     <t>A few ideas about the intricacy of completing partial latin squares.</t>
   </si>
   <si>
-    <t>Processing GPS Data in Python</t>
-  </si>
-  <si>
-    <t>An [IPython][ipython] notebook presenting a statistical investigation, based on GPS data, into anomalous driving patterns among a fleet of delivery trucks</t>
-  </si>
-  <si>
-    <t>Modelling Sudoku Puzzles in Python</t>
-  </si>
-  <si>
-    <t>An updated version of {% cite davis7modeling –file mh2 %} as an IPython notebook.</t>
-  </si>
-  <si>
-    <t>Speech Annotation in Python Using Regular Expressions</t>
-  </si>
-  <si>
-    <t>An IPython notebook which illustrates some basic ideas about annotating a corpus of novels using regular expressions.</t>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_09_15_intricacy.pdf</t>
   </si>
   <si>
     <t>On the Completability of Kite-Form Partial Latin Squares</t>
@@ -92,10 +107,7 @@
     <t>An article about completing KF-SPLS. A theorem is presented which characterises completable bound, untethered KF-SPLS of even order.</t>
   </si>
   <si>
-    <t>List-colouring in Python with Vizing</t>
-  </si>
-  <si>
-    <t>An IPython notebook introducing list-colouring of graphs using the [Vizing][vizinghome] package.</t>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_06_20_kiteform.pdf</t>
   </si>
   <si>
     <t>On Pandiagonal Strongly-Symmetric Self-Orthogonal Diagonal Latin Squares</t>
@@ -104,16 +116,25 @@
     <t>A very short article describing the discovery of a PSSSODLS of order 9.</t>
   </si>
   <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_04_16_psssodls.pdf</t>
+  </si>
+  <si>
     <t>Constraint Modelling of Pandiagonal Strongly-Symmetric Self-Orthogonal Diagonal Latin Squares</t>
   </si>
   <si>
     <t>A short article which describes how to use the constraint modelling language Essence' to describe PSSSODLS and how to use the tools Savile Row and Minion to translate those descriptions into concrete models and solve them. A comparison of automated and custom models is presented.</t>
   </si>
   <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/11_12_08_constraint_psssodls.pdf</t>
+  </si>
+  <si>
     <t>A Brief Introduction to Goldberg's Conjecture</t>
   </si>
   <si>
     <t xml:space="preserve">Notes  on Goldberg's conjecture on edge-colouring based on the first chapter of </t>
+  </si>
+  <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/11_11_17_goldberg.pdf</t>
   </si>
 </sst>
 </file>
@@ -124,7 +145,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -135,8 +156,17 @@
     </font>
     <font/>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -157,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -165,13 +195,10 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -179,7 +206,6 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
@@ -187,28 +213,43 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -511,132 +552,156 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="57.0"/>
     <col customWidth="1" min="2" max="2" width="56.14"/>
+    <col customWidth="1" min="3" max="3" width="25.14"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="12">
+      <c r="A4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="16">
         <v>43720.0</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="12">
+      <c r="A5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="16">
         <v>43658.0</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="12">
+      <c r="A6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="16">
         <v>43567.0</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17">
+      <c r="A7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="20">
         <v>43810.0</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17">
+      <c r="A8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="20">
         <v>43780.0</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="12">
-      <c r="A12" s="18"/>
+      <c r="A12" s="21"/>
     </row>
     <row r="16">
-      <c r="A16" s="18"/>
+      <c r="A16" s="21"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
+    <hyperlink r:id="rId4" ref="C5"/>
+    <hyperlink r:id="rId5" ref="C6"/>
+    <hyperlink r:id="rId6" ref="C7"/>
+    <hyperlink r:id="rId7" ref="C8"/>
+  </hyperlinks>
+  <drawing r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -676,100 +741,100 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="6">
+        <v>43510.0</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="8">
-        <v>43510.0</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="7">
+        <v>43782.0</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6">
+        <v>43721.0</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="9">
-        <v>43782.0</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="6">
+        <v>43690.0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6">
+        <v>43659.0</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8">
-        <v>43721.0</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="8">
-        <v>43690.0</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8">
-        <v>43659.0</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8">
+      <c r="C8" s="8"/>
+      <c r="D8" s="6">
         <v>43568.0</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>